<commit_message>
finished sqlite caching and testing
</commit_message>
<xml_diff>
--- a/Project Plan (Recovered).xlsx
+++ b/Project Plan (Recovered).xlsx
@@ -20,10 +20,9 @@
     <sheet name="Week 5" sheetId="6" r:id="rId6"/>
     <sheet name="week 6" sheetId="7" r:id="rId7"/>
     <sheet name="Week 7" sheetId="8" r:id="rId8"/>
-    <sheet name="Sheet2" sheetId="9" r:id="rId9"/>
+    <sheet name="week 8" sheetId="9" r:id="rId9"/>
   </sheets>
   <calcPr calcId="171027" concurrentCalc="0"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -36,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="123">
   <si>
     <t>Requirements</t>
   </si>
@@ -411,7 +410,13 @@
     <t>started work on sqlite caching</t>
   </si>
   <si>
-    <t>still working on sqlite</t>
+    <t>working on sqlite caching, almost finished. Diffculties dynamically creating tables at run time and only reading and writing when necessary</t>
+  </si>
+  <si>
+    <t>finished sqlite caching</t>
+  </si>
+  <si>
+    <t>tested sqlite caching</t>
   </si>
 </sst>
 </file>
@@ -1893,10 +1898,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:C5"/>
+  <dimension ref="B3:C9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1919,7 +1924,36 @@
         <v>42815</v>
       </c>
       <c r="C5" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="6" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B6" s="7">
+        <v>42816</v>
+      </c>
+      <c r="C6" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="7" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B7" s="7">
+        <v>42817</v>
+      </c>
+      <c r="C7" t="s">
         <v>120</v>
+      </c>
+    </row>
+    <row r="8" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B8" s="7">
+        <v>42818</v>
+      </c>
+      <c r="C8" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="9" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="C9" t="s">
+        <v>122</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
async for graph building
</commit_message>
<xml_diff>
--- a/Project Plan (Recovered).xlsx
+++ b/Project Plan (Recovered).xlsx
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="124">
   <si>
     <t>Requirements</t>
   </si>
@@ -417,6 +417,9 @@
   </si>
   <si>
     <t>tested sqlite caching</t>
+  </si>
+  <si>
+    <t>doing graph work on separte thread https://medium.com/@haarman.niek/a-dive-into-async-await-on-android-5a6699029aa3#.hmln6nn00</t>
   </si>
 </sst>
 </file>
@@ -1898,10 +1901,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:C9"/>
+  <dimension ref="B3:C11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1956,6 +1959,19 @@
         <v>122</v>
       </c>
     </row>
+    <row r="10" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B10" s="7">
+        <v>42819</v>
+      </c>
+    </row>
+    <row r="11" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B11" s="7">
+        <v>42820</v>
+      </c>
+      <c r="C11" t="s">
+        <v>123</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>